<commit_message>
Cambios en el fichero de segumiento
</commit_message>
<xml_diff>
--- a/Gestion/Seguimiento Servidor.xlsx
+++ b/Gestion/Seguimiento Servidor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertomurrodrigo/Documents/dg/PS01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertomurrodrigo/Documents/dg/PS01/Gestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDAEDB8-21E3-D44A-81A4-E367BF3AF2CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A60689-F76C-A443-AF72-1583E08CF531}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{7A36FABD-6146-3847-9A4F-6E9585A71A8E}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14720" xr2:uid="{7A36FABD-6146-3847-9A4F-6E9585A71A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Tarea</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Terminada</t>
   </si>
   <si>
-    <t>Creación de clases de prueba</t>
-  </si>
-  <si>
     <t>Creación de una clase fachada</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Creación de las clases que tanto la aplicación web como la aplicación Android usarán para proporcionar la funcionalidad especificada de la aplicación.</t>
   </si>
   <si>
-    <t>Creación y prueba de las funciones contenidas en las clases DAO descritas anteriormente.</t>
-  </si>
-  <si>
     <t>Instalación del SGBD MySQL en el servidor (el entorno Java y el servidor de aplicaciones Apache Tomcat ya estaban instalados).</t>
   </si>
   <si>
@@ -88,6 +82,60 @@
   </si>
   <si>
     <t>Configuración del SGBD MySQL (principalmente usuarios admitidos) y del servidor de aplicaciones Apache Tomcat.</t>
+  </si>
+  <si>
+    <t>Creación de clases de prueba I</t>
+  </si>
+  <si>
+    <t>Creación de clases de prueba II</t>
+  </si>
+  <si>
+    <t>Creación de pruebas para las funciones contenidas en las clases DAO descritas anteriormente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creación de pruebas para los servlets. </t>
+  </si>
+  <si>
+    <t>Tiempo estimado</t>
+  </si>
+  <si>
+    <t>1 hora</t>
+  </si>
+  <si>
+    <t>1 hora y 15 minutos</t>
+  </si>
+  <si>
+    <t>5 minutos</t>
+  </si>
+  <si>
+    <t>Pruebas de tablas para la BD</t>
+  </si>
+  <si>
+    <t>Prueba del fichero con extensión SQL de creación de tablas de la BD.</t>
+  </si>
+  <si>
+    <t>1 minuto</t>
+  </si>
+  <si>
+    <t>5 horas</t>
+  </si>
+  <si>
+    <t>1 hora y 30 minutos</t>
+  </si>
+  <si>
+    <t>4 horas</t>
+  </si>
+  <si>
+    <t>30 minutos</t>
+  </si>
+  <si>
+    <t>Tiempo real (aproximado)</t>
+  </si>
+  <si>
+    <t>Adaptación de los servlets al formato JSON</t>
+  </si>
+  <si>
+    <t>Los servlets se adaptarán para que puedan servir tanto para la aplicación web como para la aplicación Android.</t>
   </si>
 </sst>
 </file>
@@ -448,20 +496,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19ECBE5F-40C8-9A46-9E29-DEA632A8665B}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="126.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +521,14 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -480,84 +536,174 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>